<commit_message>
lupa kalo harus masukin hasil ss juga
</commit_message>
<xml_diff>
--- a/dbMysql/tugas1-normalisasi.xlsx
+++ b/dbMysql/tugas1-normalisasi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\msibPhp\materi_msib_htp\dbMysql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33DE688B-4C11-49F4-B6E7-5B7DE49EB9EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB7885C-E98F-4802-BB0B-D921A263C870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="10440" windowHeight="10890" xr2:uid="{2000A2ED-06B4-40AB-B0B6-27CD72B89542}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{2000A2ED-06B4-40AB-B0B6-27CD72B89542}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -291,7 +291,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -302,13 +302,10 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -625,10 +622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{127DFAF3-B144-4A2D-9014-450C62D7BC0A}">
-  <dimension ref="B2:M60"/>
+  <dimension ref="B2:Y37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B26" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="L43" sqref="L43"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AC31" sqref="AC31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -645,23 +642,33 @@
     <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.453125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="11.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B2" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-    </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+    </row>
+    <row r="3" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>38</v>
       </c>
@@ -693,7 +700,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B4" s="2">
         <v>1</v>
       </c>
@@ -725,7 +732,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
@@ -757,7 +764,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
@@ -789,7 +796,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B7" s="2">
         <v>2</v>
       </c>
@@ -821,7 +828,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
@@ -853,7 +860,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B9" s="2">
         <v>3</v>
       </c>
@@ -885,7 +892,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B10" s="2">
         <v>4</v>
       </c>
@@ -917,7 +924,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B11" s="2">
         <v>5</v>
       </c>
@@ -949,7 +956,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B12" s="2" t="s">
         <v>4</v>
       </c>
@@ -981,12 +988,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B15" s="1" t="s">
         <v>38</v>
       </c>
@@ -1017,8 +1024,11 @@
       <c r="K15" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="O15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B16" s="2">
         <v>1</v>
       </c>
@@ -1049,8 +1059,17 @@
       <c r="K16" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="O16" t="s">
+        <v>56</v>
+      </c>
+      <c r="R16" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="U16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B17" s="2">
         <v>1</v>
       </c>
@@ -1081,8 +1100,29 @@
       <c r="K17" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="O17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="S17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="U17" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="V17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="W17" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B18" s="2">
         <v>1</v>
       </c>
@@ -1113,8 +1153,29 @@
       <c r="K18" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="O18" s="2">
+        <v>1</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="R18" s="2">
+        <v>1</v>
+      </c>
+      <c r="S18" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="U18" s="2">
+        <v>1</v>
+      </c>
+      <c r="V18" s="2">
+        <v>2</v>
+      </c>
+      <c r="W18" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B19" s="2">
         <v>2</v>
       </c>
@@ -1145,8 +1206,29 @@
       <c r="K19" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="O19" s="2">
+        <v>2</v>
+      </c>
+      <c r="P19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="R19" s="2">
+        <v>2</v>
+      </c>
+      <c r="S19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="U19" s="2">
+        <v>2</v>
+      </c>
+      <c r="V19" s="2">
+        <v>3</v>
+      </c>
+      <c r="W19" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B20" s="2">
         <v>2</v>
       </c>
@@ -1177,8 +1259,29 @@
       <c r="K20" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="O20" s="2">
+        <v>3</v>
+      </c>
+      <c r="P20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="R20" s="2">
+        <v>3</v>
+      </c>
+      <c r="S20" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="U20" s="2">
+        <v>3</v>
+      </c>
+      <c r="V20" s="2">
+        <v>2</v>
+      </c>
+      <c r="W20" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B21" s="2">
         <v>3</v>
       </c>
@@ -1209,8 +1312,23 @@
       <c r="K21" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="R21" s="2">
+        <v>4</v>
+      </c>
+      <c r="S21" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="U21" s="2">
+        <v>4</v>
+      </c>
+      <c r="V21" s="2">
+        <v>1</v>
+      </c>
+      <c r="W21" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B22" s="2">
         <v>4</v>
       </c>
@@ -1241,8 +1359,17 @@
       <c r="K22" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="U22" s="2">
+        <v>5</v>
+      </c>
+      <c r="V22" s="2">
+        <v>4</v>
+      </c>
+      <c r="W22" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B23" s="2">
         <v>5</v>
       </c>
@@ -1273,8 +1400,17 @@
       <c r="K23" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="U23" s="2">
+        <v>6</v>
+      </c>
+      <c r="V23" s="2">
+        <v>4</v>
+      </c>
+      <c r="W23" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B24" s="2">
         <v>5</v>
       </c>
@@ -1305,21 +1441,71 @@
       <c r="K24" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="U24" s="2">
+        <v>7</v>
+      </c>
+      <c r="V24" s="2">
+        <v>3</v>
+      </c>
+      <c r="W24" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="U25" s="4"/>
+      <c r="V25" s="4"/>
+      <c r="W25" s="4"/>
+    </row>
+    <row r="26" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="O26" t="s">
+        <v>63</v>
+      </c>
+      <c r="U26" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>54</v>
       </c>
       <c r="H27" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="O27" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="P27" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="R27" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="S27" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="U27" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="V27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="W27" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X27" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y27" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B28" s="1" t="s">
         <v>38</v>
       </c>
@@ -1353,8 +1539,38 @@
       <c r="M28" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="O28" s="2">
+        <v>1</v>
+      </c>
+      <c r="P28" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q28" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="R28" s="2">
+        <v>1</v>
+      </c>
+      <c r="S28" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="U28" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="V28" s="3">
+        <v>39448</v>
+      </c>
+      <c r="W28" s="3">
+        <v>39452</v>
+      </c>
+      <c r="X28" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y28" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B29" s="2">
         <v>1</v>
       </c>
@@ -1388,8 +1604,38 @@
       <c r="M29" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="O29" s="2">
+        <v>1</v>
+      </c>
+      <c r="P29" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q29" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R29" s="2">
+        <v>1</v>
+      </c>
+      <c r="S29" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="U29" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="V29" s="3">
+        <v>39819</v>
+      </c>
+      <c r="W29" s="3">
+        <v>40653</v>
+      </c>
+      <c r="X29" s="2">
+        <v>2</v>
+      </c>
+      <c r="Y29" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B30" s="2">
         <v>1</v>
       </c>
@@ -1423,8 +1669,38 @@
       <c r="M30" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="O30" s="2">
+        <v>1</v>
+      </c>
+      <c r="P30" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q30" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="R30" s="2">
+        <v>1</v>
+      </c>
+      <c r="S30" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="U30" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="V30" s="3">
+        <v>40654</v>
+      </c>
+      <c r="W30" s="3">
+        <v>42003</v>
+      </c>
+      <c r="X30" s="2">
+        <v>3</v>
+      </c>
+      <c r="Y30" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B31" s="2">
         <v>1</v>
       </c>
@@ -1458,8 +1734,38 @@
       <c r="M31" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="O31" s="2">
+        <v>2</v>
+      </c>
+      <c r="P31" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q31" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="R31" s="2">
+        <v>1</v>
+      </c>
+      <c r="S31" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="U31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="V31" s="3">
+        <v>40179</v>
+      </c>
+      <c r="W31" s="3">
+        <v>40543</v>
+      </c>
+      <c r="X31" s="2">
+        <v>4</v>
+      </c>
+      <c r="Y31" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B32" s="2">
         <v>2</v>
       </c>
@@ -1493,8 +1799,38 @@
       <c r="M32" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="O32" s="2">
+        <v>2</v>
+      </c>
+      <c r="P32" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q32" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="R32" s="2">
+        <v>1</v>
+      </c>
+      <c r="S32" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="U32" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="V32" s="3">
+        <v>40544</v>
+      </c>
+      <c r="W32" s="3">
+        <v>40908</v>
+      </c>
+      <c r="X32" s="2">
+        <v>3</v>
+      </c>
+      <c r="Y32" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B33" s="2">
         <v>2</v>
       </c>
@@ -1528,8 +1864,38 @@
       <c r="M33" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="O33" s="2">
+        <v>3</v>
+      </c>
+      <c r="P33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q33" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="R33" s="2">
+        <v>3</v>
+      </c>
+      <c r="S33" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="U33" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="V33" s="3">
+        <v>40544</v>
+      </c>
+      <c r="W33" s="3">
+        <v>41274</v>
+      </c>
+      <c r="X33" s="2">
+        <v>5</v>
+      </c>
+      <c r="Y33" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B34" s="2">
         <v>3</v>
       </c>
@@ -1563,8 +1929,38 @@
       <c r="M34" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="O34" s="2">
+        <v>4</v>
+      </c>
+      <c r="P34" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="R34" s="2">
+        <v>2</v>
+      </c>
+      <c r="S34" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="U34" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="V34" s="3">
+        <v>40544</v>
+      </c>
+      <c r="W34" s="3">
+        <v>41274</v>
+      </c>
+      <c r="X34" s="2">
+        <v>3</v>
+      </c>
+      <c r="Y34" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B35" s="2">
         <v>4</v>
       </c>
@@ -1598,8 +1994,38 @@
       <c r="M35" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="O35" s="2">
+        <v>5</v>
+      </c>
+      <c r="P35" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q35" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="R35" s="2">
+        <v>2</v>
+      </c>
+      <c r="S35" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="U35" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="V35" s="3">
+        <v>39814</v>
+      </c>
+      <c r="W35" s="3">
+        <v>40543</v>
+      </c>
+      <c r="X35" s="2">
+        <v>6</v>
+      </c>
+      <c r="Y35" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B36" s="2">
         <v>5</v>
       </c>
@@ -1633,8 +2059,38 @@
       <c r="M36" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="O36" s="2">
+        <v>5</v>
+      </c>
+      <c r="P36" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q36" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="R36" s="2">
+        <v>2</v>
+      </c>
+      <c r="S36" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="U36" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="V36" s="3">
+        <v>40179</v>
+      </c>
+      <c r="W36" s="3">
+        <v>40908</v>
+      </c>
+      <c r="X36" s="2">
+        <v>7</v>
+      </c>
+      <c r="Y36" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B37" s="2">
         <v>5</v>
       </c>
@@ -1667,497 +2123,6 @@
       </c>
       <c r="M37" s="2" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B39" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B40" t="s">
-        <v>56</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="H40" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B41" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="I41" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="J41" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B42" s="2">
-        <v>1</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E42" s="2">
-        <v>1</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H42" s="2">
-        <v>1</v>
-      </c>
-      <c r="I42" s="2">
-        <v>2</v>
-      </c>
-      <c r="J42" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B43" s="2">
-        <v>2</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E43" s="2">
-        <v>2</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H43" s="2">
-        <v>2</v>
-      </c>
-      <c r="I43" s="2">
-        <v>3</v>
-      </c>
-      <c r="J43" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B44" s="2">
-        <v>3</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E44" s="2">
-        <v>3</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="H44" s="2">
-        <v>3</v>
-      </c>
-      <c r="I44" s="2">
-        <v>2</v>
-      </c>
-      <c r="J44" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="E45" s="2">
-        <v>4</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="H45" s="2">
-        <v>4</v>
-      </c>
-      <c r="I45" s="2">
-        <v>1</v>
-      </c>
-      <c r="J45" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="46" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="H46" s="2">
-        <v>5</v>
-      </c>
-      <c r="I46" s="2">
-        <v>4</v>
-      </c>
-      <c r="J46" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="H47" s="2">
-        <v>6</v>
-      </c>
-      <c r="I47" s="2">
-        <v>4</v>
-      </c>
-      <c r="J47" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="H48" s="2">
-        <v>7</v>
-      </c>
-      <c r="I48" s="2">
-        <v>3</v>
-      </c>
-      <c r="J48" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="49" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="H49" s="6"/>
-      <c r="I49" s="6"/>
-      <c r="J49" s="6"/>
-    </row>
-    <row r="50" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B50" t="s">
-        <v>63</v>
-      </c>
-      <c r="I50" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="51" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B51" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I51" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J51" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="K51" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="L51" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="M51" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="52" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B52" s="2">
-        <v>1</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E52" s="2">
-        <v>1</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I52" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J52" s="3">
-        <v>39448</v>
-      </c>
-      <c r="K52" s="3">
-        <v>39452</v>
-      </c>
-      <c r="L52" s="2">
-        <v>1</v>
-      </c>
-      <c r="M52" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B53" s="2">
-        <v>1</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E53" s="2">
-        <v>1</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I53" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J53" s="3">
-        <v>39819</v>
-      </c>
-      <c r="K53" s="3">
-        <v>40653</v>
-      </c>
-      <c r="L53" s="2">
-        <v>2</v>
-      </c>
-      <c r="M53" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B54" s="2">
-        <v>1</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E54" s="2">
-        <v>1</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I54" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J54" s="3">
-        <v>40654</v>
-      </c>
-      <c r="K54" s="3">
-        <v>42003</v>
-      </c>
-      <c r="L54" s="2">
-        <v>3</v>
-      </c>
-      <c r="M54" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B55" s="2">
-        <v>2</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E55" s="2">
-        <v>1</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I55" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J55" s="3">
-        <v>40179</v>
-      </c>
-      <c r="K55" s="3">
-        <v>40543</v>
-      </c>
-      <c r="L55" s="2">
-        <v>4</v>
-      </c>
-      <c r="M55" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B56" s="2">
-        <v>2</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E56" s="2">
-        <v>1</v>
-      </c>
-      <c r="F56" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I56" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J56" s="3">
-        <v>40544</v>
-      </c>
-      <c r="K56" s="3">
-        <v>40908</v>
-      </c>
-      <c r="L56" s="2">
-        <v>3</v>
-      </c>
-      <c r="M56" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B57" s="2">
-        <v>3</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E57" s="2">
-        <v>3</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I57" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J57" s="3">
-        <v>40544</v>
-      </c>
-      <c r="K57" s="3">
-        <v>41274</v>
-      </c>
-      <c r="L57" s="2">
-        <v>5</v>
-      </c>
-      <c r="M57" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="58" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B58" s="2">
-        <v>4</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E58" s="2">
-        <v>2</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I58" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J58" s="3">
-        <v>40544</v>
-      </c>
-      <c r="K58" s="3">
-        <v>41274</v>
-      </c>
-      <c r="L58" s="2">
-        <v>3</v>
-      </c>
-      <c r="M58" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="59" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B59" s="2">
-        <v>5</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E59" s="2">
-        <v>2</v>
-      </c>
-      <c r="F59" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I59" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J59" s="3">
-        <v>39814</v>
-      </c>
-      <c r="K59" s="3">
-        <v>40543</v>
-      </c>
-      <c r="L59" s="2">
-        <v>6</v>
-      </c>
-      <c r="M59" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="60" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B60" s="2">
-        <v>5</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E60" s="2">
-        <v>2</v>
-      </c>
-      <c r="F60" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I60" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J60" s="3">
-        <v>40179</v>
-      </c>
-      <c r="K60" s="3">
-        <v>40908</v>
-      </c>
-      <c r="L60" s="2">
-        <v>7</v>
-      </c>
-      <c r="M60" s="2">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>